<commit_message>
First Compression experiments ran
</commit_message>
<xml_diff>
--- a/data/tallymer/kmer_count.xlsx
+++ b/data/tallymer/kmer_count.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19020" windowHeight="13620" tabRatio="702" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19020" windowHeight="13620" tabRatio="702" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Genome_Information" sheetId="8" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="TotalKmer_graph_log" sheetId="12" r:id="rId6"/>
     <sheet name="Missing_graph_log" sheetId="11" r:id="rId7"/>
     <sheet name="32bit_KmerCount" sheetId="13" r:id="rId8"/>
+    <sheet name="Compression" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="95">
   <si>
     <t>K</t>
   </si>
@@ -174,6 +175,138 @@
   </si>
   <si>
     <t>hg19_h</t>
+  </si>
+  <si>
+    <t>chr10.fa</t>
+  </si>
+  <si>
+    <t>chr10.fa.bzip2</t>
+  </si>
+  <si>
+    <t>chr10.fa.gzip</t>
+  </si>
+  <si>
+    <t>chr10.fa.xz</t>
+  </si>
+  <si>
+    <t>chr10_h.fa</t>
+  </si>
+  <si>
+    <t>chr10_h.fa.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_h.fa.gzip</t>
+  </si>
+  <si>
+    <t>chr10_h.fa.xz</t>
+  </si>
+  <si>
+    <t>chr10_mk.fa</t>
+  </si>
+  <si>
+    <t>chr10_mk.fa.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_mk.fa.gzip</t>
+  </si>
+  <si>
+    <t>chr10_mk.fa.xz</t>
+  </si>
+  <si>
+    <t>chr10_ry.fa</t>
+  </si>
+  <si>
+    <t>chr10_ry.fa.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_ry.fa.gzip</t>
+  </si>
+  <si>
+    <t>chr10_ry.fa.xz</t>
+  </si>
+  <si>
+    <t>chr10_sw.fa</t>
+  </si>
+  <si>
+    <t>chr10_sw.fa.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_sw.fa.gzip</t>
+  </si>
+  <si>
+    <t>chr10_sw.fa.xz</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Compression_Ratio</t>
+  </si>
+  <si>
+    <t>ASCII Encoding</t>
+  </si>
+  <si>
+    <t>chr10.bit</t>
+  </si>
+  <si>
+    <t>chr10.bit.bzip2</t>
+  </si>
+  <si>
+    <t>chr10.bit.gzip</t>
+  </si>
+  <si>
+    <t>chr10.bit.xz</t>
+  </si>
+  <si>
+    <t>chr10_h.bit</t>
+  </si>
+  <si>
+    <t>chr10_h.bit.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_h.bit.gzip</t>
+  </si>
+  <si>
+    <t>chr10_h.bit.xz</t>
+  </si>
+  <si>
+    <t>chr10_mk.bit</t>
+  </si>
+  <si>
+    <t>chr10_mk.bit.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_mk.bit.gzip</t>
+  </si>
+  <si>
+    <t>chr10_mk.bit.xz</t>
+  </si>
+  <si>
+    <t>chr10_ry.bit</t>
+  </si>
+  <si>
+    <t>chr10_ry.bit.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_ry.bit.gzip</t>
+  </si>
+  <si>
+    <t>chr10_ry.bit.xz</t>
+  </si>
+  <si>
+    <t>chr10_sw.bit</t>
+  </si>
+  <si>
+    <t>chr10_sw.bit.bzip2</t>
+  </si>
+  <si>
+    <t>chr10_sw.bit.gzip</t>
+  </si>
+  <si>
+    <t>chr10_sw.bit.xz</t>
+  </si>
+  <si>
+    <t>Binary Encoding</t>
   </si>
 </sst>
 </file>
@@ -350,7 +483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -373,6 +506,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3875,11 +4009,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196390912"/>
-        <c:axId val="196392832"/>
+        <c:axId val="196456448"/>
+        <c:axId val="196458368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196390912"/>
+        <c:axId val="196456448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="64"/>
@@ -3907,21 +4041,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196392832"/>
+        <c:crossAx val="196458368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8"/>
         <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196392832"/>
+        <c:axId val="196458368"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3965,14 +4098,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196390912"/>
+        <c:crossAx val="196456448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6348,11 +6480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196220800"/>
-        <c:axId val="196227072"/>
+        <c:axId val="196291200"/>
+        <c:axId val="196297472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196220800"/>
+        <c:axId val="196291200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="44"/>
@@ -6381,21 +6513,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196227072"/>
+        <c:crossAx val="196297472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
         <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196227072"/>
+        <c:axId val="196297472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="700000000"/>
@@ -6439,14 +6570,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196220800"/>
+        <c:crossAx val="196291200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -8196,11 +8326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196842624"/>
-        <c:axId val="196844544"/>
+        <c:axId val="196751744"/>
+        <c:axId val="196753664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196842624"/>
+        <c:axId val="196751744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="48"/>
@@ -8229,21 +8359,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196844544"/>
+        <c:crossAx val="196753664"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
         <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196844544"/>
+        <c:axId val="196753664"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -8283,7 +8412,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196842624"/>
+        <c:crossAx val="196751744"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10049,11 +10178,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196279680"/>
-        <c:axId val="196687360"/>
+        <c:axId val="196511616"/>
+        <c:axId val="196521984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196279680"/>
+        <c:axId val="196511616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -10081,21 +10210,20 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196687360"/>
+        <c:crossAx val="196521984"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="4"/>
         <c:minorUnit val="2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196687360"/>
+        <c:axId val="196521984"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -10139,14 +10267,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196279680"/>
+        <c:crossAx val="196511616"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17539,11 +17666,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196590592"/>
-        <c:axId val="196592768"/>
+        <c:axId val="196729088"/>
+        <c:axId val="196731264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196590592"/>
+        <c:axId val="196729088"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -17571,21 +17698,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196592768"/>
+        <c:crossAx val="196731264"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196592768"/>
+        <c:axId val="196731264"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -17621,7 +17746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196590592"/>
+        <c:crossAx val="196729088"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -27603,7 +27728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
@@ -27648,8 +27773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S61" sqref="S61"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32789,4 +32914,580 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>133190688</v>
+      </c>
+      <c r="C3">
+        <f>B3/B3</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="22"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>36475036</v>
+      </c>
+      <c r="C4">
+        <f>B3/B4</f>
+        <v>3.6515574103888477</v>
+      </c>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5">
+        <v>39559214</v>
+      </c>
+      <c r="C5">
+        <f>B3/B5</f>
+        <v>3.3668689170619013</v>
+      </c>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>32561152</v>
+      </c>
+      <c r="C6">
+        <f>B3/B6</f>
+        <v>4.0904783712812129</v>
+      </c>
+      <c r="H6" s="22"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7">
+        <v>133190688</v>
+      </c>
+      <c r="C7">
+        <f>B7/B7</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8">
+        <v>16617129</v>
+      </c>
+      <c r="C8">
+        <f>B7/B8</f>
+        <v>8.0152647307486156</v>
+      </c>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9">
+        <v>20231126</v>
+      </c>
+      <c r="C9">
+        <f>B7/B9</f>
+        <v>6.5834540301909046</v>
+      </c>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10">
+        <v>14816516</v>
+      </c>
+      <c r="C10">
+        <f>B7/B10</f>
+        <v>8.9893391941803316</v>
+      </c>
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11">
+        <v>133190688</v>
+      </c>
+      <c r="C11">
+        <f>B11/B11</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>22982657</v>
+      </c>
+      <c r="C12">
+        <f>B11/B12</f>
+        <v>5.7952693633290533</v>
+      </c>
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>24013369</v>
+      </c>
+      <c r="C13">
+        <f>B11/B13</f>
+        <v>5.546522355942642</v>
+      </c>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>18682512</v>
+      </c>
+      <c r="C14">
+        <f>B11/B14</f>
+        <v>7.1291637869682623</v>
+      </c>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>133190688</v>
+      </c>
+      <c r="C15">
+        <f>B15/B15</f>
+        <v>1</v>
+      </c>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>22080751</v>
+      </c>
+      <c r="C16">
+        <f>B15/B16</f>
+        <v>6.0319817926482662</v>
+      </c>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>23786189</v>
+      </c>
+      <c r="C17">
+        <f>B15/B17</f>
+        <v>5.5994967499837829</v>
+      </c>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18">
+        <v>17769008</v>
+      </c>
+      <c r="C18">
+        <f>B15/B18</f>
+        <v>7.4956738158933804</v>
+      </c>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>133190688</v>
+      </c>
+      <c r="C19">
+        <f>B19/B19</f>
+        <v>1</v>
+      </c>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20">
+        <v>22161976</v>
+      </c>
+      <c r="C20">
+        <f>B19/B20</f>
+        <v>6.0098742097726303</v>
+      </c>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21">
+        <v>23702722</v>
+      </c>
+      <c r="C21">
+        <f>B19/B21</f>
+        <v>5.619214873295987</v>
+      </c>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22">
+        <v>18187388</v>
+      </c>
+      <c r="C22">
+        <f>B19/B22</f>
+        <v>7.3232444372990777</v>
+      </c>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26">
+        <v>32828686</v>
+      </c>
+      <c r="C26">
+        <f>B26/B26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>31232508</v>
+      </c>
+      <c r="C27">
+        <f>B26/B27</f>
+        <v>1.0511063024461564</v>
+      </c>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28">
+        <v>31302823</v>
+      </c>
+      <c r="C28">
+        <f>B26/B28</f>
+        <v>1.0487452201994689</v>
+      </c>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29">
+        <v>29373000</v>
+      </c>
+      <c r="C29">
+        <f>B26/B29</f>
+        <v>1.1176483845708645</v>
+      </c>
+      <c r="H29" s="22"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30">
+        <v>16414344</v>
+      </c>
+      <c r="C30">
+        <f>B30/B30</f>
+        <v>1</v>
+      </c>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31">
+        <v>13275813</v>
+      </c>
+      <c r="C31">
+        <f>B30/B31</f>
+        <v>1.2364097023662506</v>
+      </c>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32">
+        <v>12684403</v>
+      </c>
+      <c r="C32">
+        <f>B30/B32</f>
+        <v>1.2940572764835681</v>
+      </c>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33">
+        <v>11511956</v>
+      </c>
+      <c r="C33">
+        <f>B30/B33</f>
+        <v>1.4258518708723349</v>
+      </c>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34">
+        <v>16414344</v>
+      </c>
+      <c r="C34">
+        <f>B34/B34</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="22"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35">
+        <v>16318994</v>
+      </c>
+      <c r="C35">
+        <f>B34/B35</f>
+        <v>1.0058428846778178</v>
+      </c>
+      <c r="H35" s="22"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36">
+        <v>16314822</v>
+      </c>
+      <c r="C36">
+        <f>B34/B36</f>
+        <v>1.0061000971999572</v>
+      </c>
+      <c r="H36" s="22"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37">
+        <v>15886272</v>
+      </c>
+      <c r="C37">
+        <f>B34/B37</f>
+        <v>1.033240775431769</v>
+      </c>
+      <c r="H37" s="22"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38">
+        <v>16414344</v>
+      </c>
+      <c r="C38">
+        <f>B38/B38</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39">
+        <v>15639416</v>
+      </c>
+      <c r="C39">
+        <f>B38/B39</f>
+        <v>1.0495496762794723</v>
+      </c>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40">
+        <v>15753561</v>
+      </c>
+      <c r="C40">
+        <f>B38/B40</f>
+        <v>1.0419449926273812</v>
+      </c>
+      <c r="H40" s="22"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41">
+        <v>14805456</v>
+      </c>
+      <c r="C41">
+        <f>B38/B41</f>
+        <v>1.1086685881204874</v>
+      </c>
+      <c r="H41" s="22"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42">
+        <v>16414344</v>
+      </c>
+      <c r="C42">
+        <f>B42/B42</f>
+        <v>1</v>
+      </c>
+      <c r="H42" s="22"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43">
+        <v>16086943</v>
+      </c>
+      <c r="C43">
+        <f>B42/B43</f>
+        <v>1.020351971160711</v>
+      </c>
+      <c r="H43" s="22"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44">
+        <v>15886961</v>
+      </c>
+      <c r="C44">
+        <f>B42/B44</f>
+        <v>1.0331959649173936</v>
+      </c>
+      <c r="H44" s="22"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45">
+        <v>15368488</v>
+      </c>
+      <c r="C45">
+        <f>B42/B45</f>
+        <v>1.0680519775270021</v>
+      </c>
+      <c r="H45" s="22"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>